<commit_message>
Fixed details of keycap sets
- SOL-20: Specify SA profile, row 3
- classic: Specify SA profile, row 3 (incorrectly specified DSA)
- classic: add 8u spacebar.  whoops.
</commit_message>
<xml_diff>
--- a/hardware/keyboard-sol/sol-20-keycaps.xlsx
+++ b/hardware/keyboard-sol/sol-20-keycaps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/vsrc/unified_retro_keyboard/hardware/keyboard-sol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B221B20-35FF-2A48-8BCE-A350FD0F5E6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA726C1-67C9-3249-850C-0A7C619146E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19100" yWindow="8980" windowWidth="52580" windowHeight="18940" xr2:uid="{417D3D49-9D1B-454A-8402-1AFEA58C4E52}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20400" xr2:uid="{417D3D49-9D1B-454A-8402-1AFEA58C4E52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="67">
   <si>
     <t>Color  (key/legend)</t>
   </si>
@@ -234,6 +232,9 @@
   </si>
   <si>
     <t>Pad print the legend with WFO color.</t>
+  </si>
+  <si>
+    <t>All keys SA Row 3</t>
   </si>
 </sst>
 </file>
@@ -289,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -318,6 +319,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -341,13 +348,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>4153210</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>115455</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -685,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B2810FE-EEDE-4E4E-8946-A645078AF9B9}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:J39"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -712,84 +719,61 @@
       <c r="C1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="7">
-        <v>43857</v>
-      </c>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="D1" s="10">
+        <v>43860</v>
+      </c>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <f>ROW() - 2</f>
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <f t="shared" ref="A4:A13" si="0">A3+1</f>
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <f t="shared" si="0"/>
+        <f>ROW() - 2</f>
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -799,7 +783,7 @@
         <v>10</v>
       </c>
       <c r="H5" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
@@ -808,7 +792,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A6:A15" si="0">A5+1</f>
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -818,7 +802,7 @@
         <v>10</v>
       </c>
       <c r="H6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>11</v>
@@ -837,7 +821,7 @@
         <v>10</v>
       </c>
       <c r="H7" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>11</v>
@@ -856,7 +840,7 @@
         <v>10</v>
       </c>
       <c r="H8" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>11</v>
@@ -875,7 +859,7 @@
         <v>10</v>
       </c>
       <c r="H9" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>11</v>
@@ -894,7 +878,7 @@
         <v>10</v>
       </c>
       <c r="H10" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
@@ -913,7 +897,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>11</v>
@@ -932,7 +916,7 @@
         <v>10</v>
       </c>
       <c r="H12" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>11</v>
@@ -948,65 +932,61 @@
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="1">
+        <v>8</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="1">
+        <v>9</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <f>A13+1</f>
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="H15" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <f t="shared" ref="A16:A32" si="1">A15+1</f>
-        <v>13</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <f t="shared" si="1"/>
+        <f>A15+1</f>
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1016,16 +996,18 @@
         <v>10</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J17" s="3"/>
+      <c r="J17" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A18:A34" si="1">A17+1</f>
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1034,20 +1016,15 @@
       <c r="C18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="3"/>
+      <c r="H18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -1061,14 +1038,12 @@
         <v>10</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -1081,15 +1056,20 @@
       <c r="C20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="D20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1103,13 +1083,13 @@
         <v>10</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1124,13 +1104,13 @@
         <v>10</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -1145,13 +1125,13 @@
         <v>10</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -1163,16 +1143,16 @@
         <v>16</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -1184,16 +1164,16 @@
         <v>16</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I25" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1208,13 +1188,13 @@
         <v>33</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I26" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -1229,13 +1209,13 @@
         <v>33</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>11</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -1249,20 +1229,15 @@
       <c r="C28" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I28" s="1"/>
-      <c r="J28" s="3"/>
+      <c r="H28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
@@ -1276,12 +1251,14 @@
         <v>33</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J29" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
@@ -1294,12 +1271,19 @@
       <c r="C30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="D30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="1"/>
       <c r="J30" s="3"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -1311,10 +1295,10 @@
         <v>16</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>14</v>
@@ -1330,10 +1314,10 @@
         <v>16</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>14</v>
@@ -1341,22 +1325,37 @@
       <c r="J32" s="3"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I33" s="1"/>
+      <c r="A33" s="1">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="J33" s="3"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <f>A32+1</f>
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>14</v>
@@ -1364,162 +1363,185 @@
       <c r="J34" s="3"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <f t="shared" ref="A35:A36" si="2">A34+1</f>
-        <v>31</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="I35" s="1"/>
       <c r="J35" s="3"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <f t="shared" si="2"/>
+        <f>A34+1</f>
         <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <f t="shared" ref="A37:A38" si="2">A36+1</f>
+        <v>33</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="1" t="s">
+      <c r="E38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I36" s="1"/>
-      <c r="J36" s="3"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I37" s="1"/>
-      <c r="J37" s="3"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G38" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="I38" s="1"/>
       <c r="J38" s="3"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="8" t="s">
+      <c r="I39" s="1"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I40" s="1"/>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-    </row>
-    <row r="40" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
-        <f>A36+1</f>
-        <v>33</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I41" s="1"/>
-      <c r="J41" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
-        <f>A41+1</f>
-        <v>34</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I42" s="1"/>
-      <c r="J42" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+    </row>
+    <row r="42" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <f>A42+1</f>
+        <f>A38+1</f>
         <v>35</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="D43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" s="1"/>
+      <c r="J43" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <f>A43+1</f>
+        <v>36</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I44" s="1"/>
+      <c r="J44" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <f>A44+1</f>
+        <v>37</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J43" s="9" t="s">
+      <c r="I45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I44" s="1"/>
-      <c r="J44" s="5"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I45" s="1"/>
-      <c r="J45" s="5"/>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I46" s="1"/>
+      <c r="J46" s="5"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I47" s="1"/>
+      <c r="J47" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A39:J39"/>
+    <mergeCell ref="A41:J41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Corrections to Sol-20 keycap BOM
- Add the _/DEL key
- Specify that the keypad "." key be centered vertically and horizontally.
</commit_message>
<xml_diff>
--- a/hardware/keyboard-sol/sol-20-keycaps.xlsx
+++ b/hardware/keyboard-sol/sol-20-keycaps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/vsrc/unified_retro_keyboard/hardware/keyboard-sol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA726C1-67C9-3249-850C-0A7C619146E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43D7CB0-E774-9546-A22E-332E0AC8802D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20400" xr2:uid="{417D3D49-9D1B-454A-8402-1AFEA58C4E52}"/>
+    <workbookView xWindow="22640" yWindow="4580" windowWidth="40780" windowHeight="34580" xr2:uid="{417D3D49-9D1B-454A-8402-1AFEA58C4E52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="70">
   <si>
     <t>Color  (key/legend)</t>
   </si>
@@ -132,9 +134,6 @@
     <t>.</t>
   </si>
   <si>
-    <t>period</t>
-  </si>
-  <si>
     <t>1.25u</t>
   </si>
   <si>
@@ -235,6 +234,18 @@
   </si>
   <si>
     <t>All keys SA Row 3</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>DEL</t>
+  </si>
+  <si>
+    <t>Top is "_" (underscore)</t>
+  </si>
+  <si>
+    <t>decimal point.  Centered vertically and horizontally in keycap.</t>
   </si>
 </sst>
 </file>
@@ -290,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -318,6 +329,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -348,13 +362,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>4153210</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>115455</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -692,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B2810FE-EEDE-4E4E-8946-A645078AF9B9}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,19 +728,19 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="10">
+        <v>63</v>
+      </c>
+      <c r="D1" s="11">
         <v>43860</v>
       </c>
-      <c r="E1" s="11"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -741,7 +755,7 @@
     </row>
     <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -792,7 +806,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <f t="shared" ref="A6:A15" si="0">A5+1</f>
+        <f t="shared" ref="A6:A16" si="0">A5+1</f>
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -970,44 +984,51 @@
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I16" s="1"/>
+      <c r="I16" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <f>A15+1</f>
-        <v>14</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <f t="shared" ref="A18:A34" si="1">A17+1</f>
+        <f>A16+1</f>
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1023,12 +1044,12 @@
         <v>14</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A19:A35" si="1">A18+1</f>
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1038,12 +1059,14 @@
         <v>10</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J19" s="3"/>
+      <c r="J19" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -1056,19 +1079,12 @@
       <c r="C20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1082,15 +1098,20 @@
       <c r="C21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="D21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -1104,13 +1125,13 @@
         <v>10</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -1125,13 +1146,13 @@
         <v>10</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -1146,13 +1167,13 @@
         <v>10</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -1167,13 +1188,13 @@
         <v>10</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1185,16 +1206,16 @@
         <v>16</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -1206,16 +1227,16 @@
         <v>16</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -1227,16 +1248,16 @@
         <v>16</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>11</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -1248,16 +1269,16 @@
         <v>16</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>11</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -1269,22 +1290,17 @@
         <v>16</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I30" s="1"/>
-      <c r="J30" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -1295,14 +1311,21 @@
         <v>16</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="1"/>
       <c r="J31" s="3"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -1314,10 +1337,10 @@
         <v>16</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>14</v>
@@ -1333,10 +1356,10 @@
         <v>16</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>14</v>
@@ -1352,52 +1375,52 @@
         <v>16</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="H34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J34" s="3"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I35" s="1"/>
+      <c r="H35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="J35" s="3"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <f>A34+1</f>
-        <v>32</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="I36" s="1"/>
       <c r="J36" s="3"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <f t="shared" ref="A37:A38" si="2">A36+1</f>
+        <f>A35+1</f>
         <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>14</v>
@@ -1406,31 +1429,46 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
+        <f t="shared" ref="A38:A39" si="2">A37+1</f>
+        <v>34</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
         <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="C39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I38" s="1"/>
-      <c r="J38" s="3"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G39" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="I39" s="1"/>
       <c r="J39" s="3"/>
     </row>
@@ -1439,51 +1477,27 @@
       <c r="J40" s="3"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-    </row>
-    <row r="42" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
-        <f>A38+1</f>
-        <v>35</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I43" s="1"/>
-      <c r="J43" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
+      <c r="I41" s="1"/>
+      <c r="J41" s="3"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+    </row>
+    <row r="43" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <f>A43+1</f>
+        <f>A39+1</f>
         <v>36</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1493,20 +1507,20 @@
         <v>15</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I44" s="1"/>
       <c r="J44" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1515,33 +1529,61 @@
         <v>37</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="D45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I45" s="1"/>
       <c r="J45" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I46" s="1"/>
-      <c r="J46" s="5"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <f>A45+1</f>
+        <v>38</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46" s="9" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I47" s="1"/>
       <c r="J47" s="5"/>
     </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I48" s="1"/>
+      <c r="J48" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A41:J41"/>
+    <mergeCell ref="A42:J42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added "HERE IS" and 1.5u TAB key to classic design
</commit_message>
<xml_diff>
--- a/hardware/keyboard-sol/sol-20-keycaps.xlsx
+++ b/hardware/keyboard-sol/sol-20-keycaps.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/vsrc/unified_retro_keyboard/hardware/keyboard-sol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43D7CB0-E774-9546-A22E-332E0AC8802D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4271B9D8-6806-FB41-89C9-55BF0209E147}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22640" yWindow="4580" windowWidth="40780" windowHeight="34580" xr2:uid="{417D3D49-9D1B-454A-8402-1AFEA58C4E52}"/>
   </bookViews>
@@ -708,7 +708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B2810FE-EEDE-4E4E-8946-A645078AF9B9}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>

</xml_diff>